<commit_message>
updated robot input patameters
</commit_message>
<xml_diff>
--- a/IDLoop_Robot_EA_20231019.xlsx
+++ b/IDLoop_Robot_EA_20231019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BIN\Mehnert\yasakawa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BIN\Mehnert\yasakawa\IdLoopGateway\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F672E6-7956-4180-9A9F-727A4A0E52C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E550E096-DC28-4A1C-9CBC-9F329077BBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Robot Inputs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="203">
   <si>
     <t>Name</t>
   </si>
@@ -569,13 +569,79 @@
   </si>
   <si>
     <t>G_FromYasakawa[24].7</t>
+  </si>
+  <si>
+    <t>Druck [N/100]</t>
+  </si>
+  <si>
+    <t>Geschwindigkeit</t>
+  </si>
+  <si>
+    <t>Weg</t>
+  </si>
+  <si>
+    <t>Fingerdurchmesser</t>
+  </si>
+  <si>
+    <t>Startoientierung</t>
+  </si>
+  <si>
+    <t>Endorientierung</t>
+  </si>
+  <si>
+    <t>X Verschiebung</t>
+  </si>
+  <si>
+    <t>Y Verschiebung</t>
+  </si>
+  <si>
+    <t>RX Offset Start</t>
+  </si>
+  <si>
+    <t>RY Offset Start</t>
+  </si>
+  <si>
+    <t>RZ Offset Start</t>
+  </si>
+  <si>
+    <t>RX Offset End</t>
+  </si>
+  <si>
+    <t>RY Offset End</t>
+  </si>
+  <si>
+    <t>Rz Offset End</t>
+  </si>
+  <si>
+    <t>Scannerverschiebung</t>
+  </si>
+  <si>
+    <t>Jobnummer???</t>
+  </si>
+  <si>
+    <t>Byte 53 .. Byte 54</t>
+  </si>
+  <si>
+    <t>Byte 55 .. Byte 56</t>
+  </si>
+  <si>
+    <t>Byte 57 .. Byte 58</t>
+  </si>
+  <si>
+    <t>Byte 59 .. Byte 60</t>
+  </si>
+  <si>
+    <t>Byte 61 .. Byte 62</t>
+  </si>
+  <si>
+    <t>Byte 63 .. Byte 64</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -585,6 +651,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -616,12 +689,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -906,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1162,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1109,8 +1185,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>53</v>
+      <c r="A14" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>56</v>
@@ -1132,8 +1208,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>51</v>
+      <c r="A15" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>57</v>
@@ -1152,8 +1228,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>58</v>
+      <c r="A16" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>59</v>
@@ -1175,8 +1251,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>62</v>
+      <c r="A17" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>63</v>
@@ -1195,8 +1271,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>65</v>
+      <c r="A18" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>66</v>
@@ -1218,8 +1294,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>68</v>
+      <c r="A19" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>77</v>
@@ -1241,8 +1317,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>70</v>
+      <c r="A20" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>79</v>
@@ -1264,8 +1340,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>84</v>
+      <c r="A21" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>78</v>
@@ -1284,8 +1360,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>85</v>
+      <c r="A22" s="3" t="s">
+        <v>189</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>80</v>
@@ -1304,8 +1380,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>86</v>
+      <c r="A23" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>81</v>
@@ -1324,8 +1400,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>87</v>
+      <c r="A24" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>82</v>
@@ -1344,8 +1420,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>88</v>
+      <c r="A25" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>83</v>
@@ -1364,38 +1440,71 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="F26" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="G26" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="F27" s="1" t="s">
         <v>169</v>
       </c>
+      <c r="G27" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>195</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>170</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>196</v>
+      </c>
       <c r="F29" s="1" t="s">
         <v>171</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F30" s="1" t="s">
         <v>172</v>
       </c>
+      <c r="G30" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F31" s="1" t="s">
         <v>173</v>
       </c>
+      <c r="G31" s="1" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F32" s="1" t="s">
         <v>174</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1408,7 +1517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404F40BB-1225-4924-87E8-AE696E86958D}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>